<commit_message>
logic for new line changed for android
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -13,21 +13,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="292">
   <si>
     <t>KEYS</t>
   </si>
   <si>
+    <t>sn</t>
+  </si>
+  <si>
     <t>japanese</t>
   </si>
   <si>
     <t>english</t>
   </si>
   <si>
-    <t>chinese</t>
-  </si>
-  <si>
-    <t>arabic</t>
+    <t>main_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DoCo22は日本に訪日している外国人に向けての
+位置情報共有アプリケーションです。
+もちろん、日本人でも使用OK。
+無料でご利用できます。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DoCo22 is a location sharing application for foreigners visiting japan.
+Also avaiable for japanese . Avaiable for free.</t>
+  </si>
+  <si>
+    <t>main_2</t>
+  </si>
+  <si>
+    <t>困ったら、DoCo22を…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When in trouble , DoCo22</t>
   </si>
   <si>
     <t>select_language</t>
@@ -42,7 +61,7 @@
     <t>select_nationality</t>
   </si>
   <si>
-    <t>国籍選び</t>
+    <t>国籍選択</t>
   </si>
   <si>
     <t xml:space="preserve">Select nationality</t>
@@ -54,7 +73,7 @@
     <t>プランの違いについて</t>
   </si>
   <si>
-    <t xml:space="preserve">About plan</t>
+    <t xml:space="preserve">About use of plan</t>
   </si>
   <si>
     <t>toc</t>
@@ -63,7 +82,7 @@
     <t>利用規約について</t>
   </si>
   <si>
-    <t xml:space="preserve">Terms and condition</t>
+    <t xml:space="preserve">Terms and conditions</t>
   </si>
   <si>
     <t>free_plan</t>
@@ -78,7 +97,7 @@
     <t>use_without_registration</t>
   </si>
   <si>
-    <t>全員登録無して利用する</t>
+    <t>会員登録無しで利用する</t>
   </si>
   <si>
     <t xml:space="preserve">Use without registration</t>
@@ -96,7 +115,7 @@
     <t>user_with_registration</t>
   </si>
   <si>
-    <t>全員登録をして利用する</t>
+    <t>会員登録をして利用する</t>
   </si>
   <si>
     <t xml:space="preserve">Use by registration</t>
@@ -120,27 +139,27 @@
     <t xml:space="preserve">Already signed up users</t>
   </si>
   <si>
-    <t>国籍選択</t>
-  </si>
-  <si>
     <t>search</t>
   </si>
   <si>
     <t>検索</t>
   </si>
   <si>
+    <t>Search</t>
+  </si>
+  <si>
     <t>next</t>
   </si>
   <si>
     <t>次へ</t>
   </si>
   <si>
+    <t>Next</t>
+  </si>
+  <si>
     <t>normal_plan_registration</t>
   </si>
   <si>
-    <t>ノーマルプラン登録</t>
-  </si>
-  <si>
     <t xml:space="preserve">Normal plan registration</t>
   </si>
   <si>
@@ -150,19 +169,25 @@
     <t>アイコン</t>
   </si>
   <si>
+    <t>Icon</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
     <t>ユーザーネーム</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
     <t>mail</t>
   </si>
   <si>
     <t>メールアドレス</t>
   </si>
   <si>
-    <t xml:space="preserve">mail address</t>
+    <t xml:space="preserve">Email address</t>
   </si>
   <si>
     <t>signup</t>
@@ -171,20 +196,731 @@
     <t>ノーマルプランに登録する</t>
   </si>
   <si>
-    <t xml:space="preserve">sign up</t>
-  </si>
-  <si>
     <t>back</t>
   </si>
   <si>
-    <t>もどる</t>
+    <t>戻る</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>signup_alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ご登録いただきましたメールアドレスに
+確認メールをお送りしました。
+メールに記載されています。
+URLをクリック後、登録完了となります。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A confirmation e-mail has been sent to your registered
+mail address.Registration is complete after clicking on 
+the URL.</t>
+  </si>
+  <si>
+    <t>signup_alert_note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">＜注意＞
+メールが届かない場合は【迷惑メールフォルダを確認】
+または、お手数ですが毛一度ご登録ください。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Note&gt;
+If you do not receive the mail, please check junk e-mail 
+folder or register once again</t>
+  </si>
+  <si>
+    <t>thankyou_for_registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">インストールしていただき
+ありがとうございます
+DoCo22はユーザー皆さまで
+作り上げていくアプリです</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for registration.</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>スキップ</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>remember_doco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">見つかりにくい場所や
+困ったことがあったら
+DoCo22にお任せ！</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When in trouble finding the places , remember DoCo22</t>
+  </si>
+  <si>
+    <t>first_phase_we_help_you_find</t>
+  </si>
+  <si>
+    <t xml:space="preserve">第１弾は【喫煙所】
+喫煙できる場所。お店を
+検索できる他、
+禁煙エリアもわかります
+それでは、アプリを
+使ってみましょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the first phase , we help you find the smoking zone and restricted areas for smoking .
+lets get started 
+</t>
+  </si>
+  <si>
+    <t>go_to_map</t>
+  </si>
+  <si>
+    <t>Mapへ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Map</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>apply_new_place</t>
+  </si>
+  <si>
+    <t>新しい場所を申請する</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply for a new location</t>
+  </si>
+  <si>
+    <t>申請</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>キャンセル</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>submit_application</t>
+  </si>
+  <si>
+    <t>投稿申請</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit application</t>
+  </si>
+  <si>
+    <t>check_in</t>
+  </si>
+  <si>
+    <t>チェックイン</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check in</t>
+  </si>
+  <si>
+    <t>2020年1月20日</t>
+  </si>
+  <si>
+    <t>2020/1/20</t>
+  </si>
+  <si>
+    <t>select_category</t>
+  </si>
+  <si>
+    <t>カテゴリ選択</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select category</t>
+  </si>
+  <si>
+    <t>喫煙所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoking zone</t>
+  </si>
+  <si>
+    <t>name_of_smoking_zone</t>
+  </si>
+  <si>
+    <t>場所の名前</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place name</t>
+  </si>
+  <si>
+    <t>例：秋葉原駅前公園横</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eg: Akihabara station square side park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">店舗内/ その他</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inside store/other</t>
+  </si>
+  <si>
+    <t>商業施設</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commercial facility</t>
+  </si>
+  <si>
+    <t>外</t>
+  </si>
+  <si>
+    <t>outdoor</t>
+  </si>
+  <si>
+    <t>喫煙できるタバコ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type of cigaratte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">紙タバコと電子タバコ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal and electronic cigaratte</t>
+  </si>
+  <si>
+    <t>電子タバコのみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electronic cigaratte only</t>
+  </si>
+  <si>
+    <t>任意項目</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optional choice</t>
+  </si>
+  <si>
+    <t>外観/写真</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appearance/ photo</t>
+  </si>
+  <si>
+    <t>住所</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>例：東京都千代田区秋葉原1－1－1－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eg:Tokyo to Chiyodaku Akihabara 1-1-1</t>
+  </si>
+  <si>
+    <t>営業時間</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open hour</t>
+  </si>
+  <si>
+    <t>24時間利用可能</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open 24hour </t>
+  </si>
+  <si>
+    <t>時間あり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time limitation</t>
+  </si>
+  <si>
+    <t>開始時間</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opening time</t>
+  </si>
+  <si>
+    <t>終了時間</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closing time</t>
+  </si>
+  <si>
+    <t>時間追加</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add time</t>
+  </si>
+  <si>
+    <t>休業日</t>
+  </si>
+  <si>
+    <t>holiday</t>
+  </si>
+  <si>
+    <t>その他</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>店舗以外の場合の情報</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information on non-store locations</t>
+  </si>
+  <si>
+    <t>屋根あり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with roof</t>
+  </si>
+  <si>
+    <t>屋根なし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">without roof</t>
+  </si>
+  <si>
+    <t>ベンチあり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with benches</t>
+  </si>
+  <si>
+    <t>ベンチなし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">without benches</t>
+  </si>
+  <si>
+    <t>囲いあり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with enclosure</t>
+  </si>
+  <si>
+    <t>囲いなし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">without enclosure</t>
+  </si>
+  <si>
+    <t>タバコ自販機あり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with vending machine for cigaratte </t>
+  </si>
+  <si>
+    <t>タバコ自販機なし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">without vending machine for cigaratte </t>
+  </si>
+  <si>
+    <t>飲料自販機あり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vending machine avaiable</t>
+  </si>
+  <si>
+    <t>飲料自販機なし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vending machine not avaiable</t>
+  </si>
+  <si>
+    <t>checkin</t>
+  </si>
+  <si>
+    <t>おめでとうございます！</t>
+  </si>
+  <si>
+    <t>congratulations!</t>
+  </si>
+  <si>
+    <t>九段下公園の小屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kudansita park</t>
+  </si>
+  <si>
+    <t>公園の中ではなく、外にありました。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was not inside the park but outside</t>
+  </si>
+  <si>
+    <t>外にあるので、雨だと要注意！</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because it's an outdoor space, be carefull during rain!</t>
+  </si>
+  <si>
+    <t>もっと読む</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read more</t>
+  </si>
+  <si>
+    <t>詳細</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>レビューを書く</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write a review</t>
+  </si>
+  <si>
+    <t>この場所では２回目ですね！</t>
+  </si>
+  <si>
+    <t xml:space="preserve">its your second visit here</t>
+  </si>
+  <si>
+    <t>お帰りなさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">welcome back</t>
+  </si>
+  <si>
+    <t>あなたが見つけた場所でしたね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was it the place you were looking for!</t>
+  </si>
+  <si>
+    <t>edit_delete</t>
+  </si>
+  <si>
+    <t>編集依頼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit request</t>
+  </si>
+  <si>
+    <t>場所の編集</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit place</t>
+  </si>
+  <si>
+    <t>追加情報などの依頼出来ます</t>
+  </si>
+  <si>
+    <t xml:space="preserve">request for additional information</t>
+  </si>
+  <si>
+    <t>削除依頼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">request for deletion</t>
+  </si>
+  <si>
+    <t>場所の削除をいらい出来ます</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you can request for deletion</t>
+  </si>
+  <si>
+    <t>ご協力ありがとうございます</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thanks for your corporation</t>
+  </si>
+  <si>
+    <t>理由</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>撤去されていた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was removed</t>
+  </si>
+  <si>
+    <t>私物だった</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was private</t>
+  </si>
+  <si>
+    <t>top_mypage_free</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>すべて</t>
+  </si>
+  <si>
+    <t>smoking_zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smoking zone</t>
+  </si>
+  <si>
+    <t>foreign_exchange</t>
+  </si>
+  <si>
+    <t>両替所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign exchange</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t>トイレ</t>
+  </si>
+  <si>
+    <t>resturant</t>
+  </si>
+  <si>
+    <t>飲食店</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resturant </t>
+  </si>
+  <si>
+    <t>dustbin</t>
+  </si>
+  <si>
+    <t>ゴミ箱</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>一覧に戻る</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back to index</t>
+  </si>
+  <si>
+    <t>top_login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email address</t>
+  </si>
+  <si>
+    <t>can_not_login</t>
+  </si>
+  <si>
+    <t>ログインできない方はコチラから</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click here if you cannot log in</t>
+  </si>
+  <si>
+    <t>new_registration</t>
+  </si>
+  <si>
+    <t>新規登録はコチラ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click here for new registration</t>
+  </si>
+  <si>
+    <t>normal_place</t>
+  </si>
+  <si>
+    <t>信頼度</t>
+  </si>
+  <si>
+    <t>credibility</t>
+  </si>
+  <si>
+    <t>最終チェックイン</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initial checkin</t>
+  </si>
+  <si>
+    <t>人</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>件</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>お気に入り</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>profile_edit</t>
+  </si>
+  <si>
+    <t>プロフィール編集</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit profile</t>
+  </si>
+  <si>
+    <t>画像変更</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit photo</t>
+  </si>
+  <si>
+    <t>使用言語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">language </t>
+  </si>
+  <si>
+    <t>日本語</t>
+  </si>
+  <si>
+    <t>国籍</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <t>japan</t>
+  </si>
+  <si>
+    <t>保存する</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>normal_review</t>
+  </si>
+  <si>
+    <t>レビュー投稿</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post review</t>
+  </si>
+  <si>
+    <t>オススメ度</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>コメント</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>例：小屋の中みたいな感じで、空気清浄機があってキレイでした。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eg: the space feels like inside a cabin, nice with air cleaner</t>
+  </si>
+  <si>
+    <t>投稿を確認</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirm </t>
+  </si>
+  <si>
+    <t>なしでもok</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>投稿者情報</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contributor information</t>
+  </si>
+  <si>
+    <t>レビューを送信</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>top_mypage_normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal plan</t>
+  </si>
+  <si>
+    <t>プロフィール変更</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit profile </t>
+  </si>
+  <si>
+    <t>プラン変更</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit plan</t>
+  </si>
+  <si>
+    <t>チェックイン履歴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkin history</t>
+  </si>
+  <si>
+    <t>追加</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>削除申請履歴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete request history</t>
+  </si>
+  <si>
+    <t>国籍を選択してください</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please select the nationality</t>
+  </si>
+  <si>
+    <t>言語を選んでください</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please select the language</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -201,14 +937,33 @@
       <color theme="1"/>
       <sz val="16"/>
     </font>
+    <font/>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill/>
     <fill/>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor theme="6" tint="0.39997558519241921"/>
       </patternFill>
     </fill>
   </fills>
@@ -231,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -239,8 +994,29 @@
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,24 +1546,24 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" ht="15.75">
+    <row r="2" ht="94.5">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -795,15 +1571,17 @@
     </row>
     <row r="3" ht="15.75">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -811,15 +1589,17 @@
     </row>
     <row r="4" ht="15.75">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -827,15 +1607,17 @@
     </row>
     <row r="5" ht="15.75">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -843,15 +1625,17 @@
     </row>
     <row r="6" ht="15.75">
       <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -859,15 +1643,17 @@
     </row>
     <row r="7" ht="15.75">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -875,15 +1661,15 @@
     </row>
     <row r="8" ht="15.75">
       <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -891,15 +1677,17 @@
     </row>
     <row r="9" ht="15.75">
       <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -907,15 +1695,15 @@
     </row>
     <row r="10" ht="15.75">
       <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -923,29 +1711,33 @@
     </row>
     <row r="11" ht="15.75">
       <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" ht="15.75">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -953,31 +1745,33 @@
     </row>
     <row r="13" ht="15.75">
       <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1"/>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" ht="15.75">
-      <c r="A14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -987,13 +1781,15 @@
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="1">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1003,13 +1799,15 @@
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1017,15 +1815,15 @@
     </row>
     <row r="17" ht="15.75">
       <c r="A17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1"/>
+      <c r="B17" s="1">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1033,15 +1831,17 @@
     </row>
     <row r="18" ht="15.75">
       <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="B18" s="1">
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1049,15 +1849,17 @@
     </row>
     <row r="19" ht="15.75">
       <c r="A19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="B19" s="1">
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1065,105 +1867,175 @@
     </row>
     <row r="20" ht="15.75">
       <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="B20" s="1">
+        <v>16</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" ht="15.75">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" ht="15.75">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" ht="15.75">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+    <row r="23" ht="94.5">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="6">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" ht="15.75">
-      <c r="A24" s="1"/>
+    <row r="24" ht="78.75">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" ht="15.75">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+    <row r="25" ht="63">
+      <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1">
+        <v>20</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" ht="15.75">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1">
+        <v>21</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" ht="15.75">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+    <row r="27" ht="47.25">
+      <c r="A27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" ht="15.75">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+    <row r="28" ht="126">
+      <c r="A28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="1">
+        <v>23</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" ht="15.75">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1172,7 +2044,9 @@
     <row r="30" ht="15.75">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1180,10 +2054,18 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" ht="15.75">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="6">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1191,39 +2073,69 @@
     </row>
     <row r="32" ht="15.75">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" ht="15.75">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="6">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" ht="15.75">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" ht="15.75">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="6">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1231,19 +2143,33 @@
     </row>
     <row r="36" ht="15.75">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="B36" s="1">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
     <row r="37" ht="15.75">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="6">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1251,19 +2177,33 @@
     </row>
     <row r="38" ht="15.75">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="B38" s="1">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" ht="15.75">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="6">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1271,9 +2211,15 @@
     </row>
     <row r="40" ht="15.75">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="B40" s="1">
+        <v>11</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1281,9 +2227,15 @@
     </row>
     <row r="41" ht="15.75">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="B41" s="6">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1291,9 +2243,15 @@
     </row>
     <row r="42" ht="15.75">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="B42" s="1">
+        <v>13</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1301,9 +2259,15 @@
     </row>
     <row r="43" ht="15.75">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="B43" s="6">
+        <v>14</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1311,9 +2275,15 @@
     </row>
     <row r="44" ht="15.75">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="B44" s="1">
+        <v>15</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -1321,9 +2291,15 @@
     </row>
     <row r="45" ht="15.75">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="B45" s="6">
+        <v>16</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1331,9 +2307,15 @@
     </row>
     <row r="46" ht="15.75">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="B46" s="1">
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1341,9 +2323,15 @@
     </row>
     <row r="47" ht="15.75">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="6">
+        <v>18</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -1351,9 +2339,15 @@
     </row>
     <row r="48" ht="15.75">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+      <c r="B48" s="1">
+        <v>19</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -1361,9 +2355,15 @@
     </row>
     <row r="49" ht="15.75">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="B49" s="6">
+        <v>20</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -1371,9 +2371,15 @@
     </row>
     <row r="50" ht="15.75">
       <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
+      <c r="B50" s="1">
+        <v>21</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -1381,9 +2387,15 @@
     </row>
     <row r="51" ht="15.75">
       <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="B51" s="6">
+        <v>22</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -1391,9 +2403,15 @@
     </row>
     <row r="52" ht="15.75">
       <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="B52" s="1">
+        <v>23</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -1401,9 +2419,15 @@
     </row>
     <row r="53" ht="15.75">
       <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="B53" s="6">
+        <v>24</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -1411,9 +2435,15 @@
     </row>
     <row r="54" ht="15.75">
       <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+      <c r="B54" s="1">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -1421,9 +2451,15 @@
     </row>
     <row r="55" ht="15.75">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="B55" s="6">
+        <v>26</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -1431,9 +2467,15 @@
     </row>
     <row r="56" ht="15.75">
       <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="B56" s="1">
+        <v>27</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -1441,9 +2483,15 @@
     </row>
     <row r="57" ht="15.75">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="B57" s="6">
+        <v>28</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -1451,9 +2499,15 @@
     </row>
     <row r="58" ht="15.75">
       <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+      <c r="B58" s="1">
+        <v>29</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -1461,9 +2515,15 @@
     </row>
     <row r="59" ht="15.75">
       <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="B59" s="6">
+        <v>30</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>147</v>
+      </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -1471,9 +2531,15 @@
     </row>
     <row r="60" ht="15.75">
       <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="B60" s="1">
+        <v>31</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -1481,9 +2547,15 @@
     </row>
     <row r="61" ht="15.75">
       <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="B61" s="6">
+        <v>32</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -1491,9 +2563,15 @@
     </row>
     <row r="62" ht="15.75">
       <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="B62" s="1">
+        <v>33</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -1501,9 +2579,15 @@
     </row>
     <row r="63" ht="15.75">
       <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+      <c r="B63" s="6">
+        <v>34</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -1511,9 +2595,15 @@
     </row>
     <row r="64" ht="15.75">
       <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="B64" s="1">
+        <v>35</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -1521,9 +2611,15 @@
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="B65" s="6">
+        <v>36</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -1531,9 +2627,15 @@
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="B66" s="1">
+        <v>37</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -1541,9 +2643,15 @@
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="B67" s="6">
+        <v>38</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -1551,9 +2659,15 @@
     </row>
     <row r="68" ht="14.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="B68" s="1">
+        <v>39</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -1561,9 +2675,15 @@
     </row>
     <row r="69" ht="14.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="B69" s="6">
+        <v>40</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -1581,8 +2701,10 @@
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -1591,9 +2713,15 @@
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -1601,9 +2729,15 @@
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="B73" s="6">
+        <v>2</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -1611,9 +2745,15 @@
     </row>
     <row r="74" ht="14.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="B74" s="1">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -1621,9 +2761,15 @@
     </row>
     <row r="75" ht="14.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
+      <c r="B75" s="1">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -1631,9 +2777,15 @@
     </row>
     <row r="76" ht="14.25">
       <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
+      <c r="B76" s="6">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -1641,9 +2793,15 @@
     </row>
     <row r="77" ht="14.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
+      <c r="B77" s="1">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -1651,9 +2809,15 @@
     </row>
     <row r="78" ht="14.25">
       <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
+      <c r="B78" s="1">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -1661,9 +2825,15 @@
     </row>
     <row r="79" ht="14.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
+      <c r="B79" s="6">
+        <v>8</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -1671,9 +2841,15 @@
     </row>
     <row r="80" ht="14.25">
       <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
+      <c r="B80" s="1">
+        <v>9</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -1681,9 +2857,15 @@
     </row>
     <row r="81" ht="14.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
+      <c r="B81" s="1">
+        <v>10</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -1701,8 +2883,10 @@
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="10" t="s">
+        <v>189</v>
+      </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -1711,9 +2895,15 @@
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -1721,9 +2911,15 @@
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
+      <c r="B85" s="6">
+        <v>2</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -1731,9 +2927,15 @@
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="B86" s="1">
+        <v>3</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -1741,9 +2943,15 @@
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
+      <c r="B87" s="1">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -1751,9 +2959,15 @@
     </row>
     <row r="88" ht="14.25">
       <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
+      <c r="B88" s="6">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -1761,9 +2975,15 @@
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
+      <c r="B89" s="1">
+        <v>6</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -1771,9 +2991,15 @@
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
+      <c r="B90" s="1">
+        <v>7</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
@@ -1781,9 +3007,15 @@
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
+      <c r="B91" s="6">
+        <v>8</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -1791,9 +3023,15 @@
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="B92" s="1">
+        <v>9</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -1812,7 +3050,9 @@
     <row r="94" ht="14.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="C94" s="10" t="s">
+        <v>208</v>
+      </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
@@ -1820,60 +3060,108 @@
       <c r="H94" s="1"/>
     </row>
     <row r="95" ht="14.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
     <row r="96" ht="14.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B96" s="6">
+        <v>2</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
     <row r="97" ht="14.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
+      <c r="A97" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B97" s="1">
+        <v>3</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
     <row r="98" ht="14.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
+      <c r="A98" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B98" s="1">
+        <v>4</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
     <row r="99" ht="14.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B99" s="6">
+        <v>5</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
     <row r="100" ht="14.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
+      <c r="A100" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B100" s="1">
+        <v>6</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
@@ -1891,8 +3179,10 @@
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -1901,9 +3191,15 @@
     </row>
     <row r="103" ht="14.25">
       <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="B103" s="1">
+        <v>1</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
@@ -1911,9 +3207,15 @@
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
+      <c r="B104" s="6">
+        <v>2</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
@@ -1932,7 +3234,9 @@
     <row r="106" ht="14.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
+      <c r="C106" s="10" t="s">
+        <v>226</v>
+      </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -1941,9 +3245,15 @@
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="B107" s="1">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
@@ -1951,29 +3261,51 @@
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="B108" s="6">
+        <v>2</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
     <row r="109" ht="14.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B109" s="1">
+        <v>3</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>230</v>
+      </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
     <row r="110" ht="14.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B110" s="1">
+        <v>4</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>233</v>
+      </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
@@ -1981,7 +3313,7 @@
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
+      <c r="B111" s="6"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -1992,7 +3324,9 @@
     <row r="112" ht="14.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
+      <c r="C112" s="10" t="s">
+        <v>234</v>
+      </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -2001,9 +3335,15 @@
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
+      <c r="B113" s="1">
+        <v>1</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
@@ -2011,9 +3351,15 @@
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
+      <c r="B114" s="6">
+        <v>2</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -2021,9 +3367,15 @@
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
+      <c r="B115" s="1">
+        <v>3</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>240</v>
+      </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
@@ -2031,9 +3383,15 @@
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
+      <c r="B116" s="1">
+        <v>4</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
@@ -2041,49 +3399,513 @@
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
+      <c r="B117" s="6">
+        <v>5</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" ht="14.25"/>
-    <row r="119" ht="14.25"/>
-    <row r="120" ht="14.25"/>
-    <row r="121" ht="14.25"/>
-    <row r="122" ht="14.25"/>
-    <row r="123" ht="14.25"/>
-    <row r="124" ht="14.25"/>
-    <row r="125" ht="14.25"/>
-    <row r="126" ht="14.25"/>
-    <row r="127" ht="14.25"/>
-    <row r="128" ht="14.25"/>
-    <row r="129" ht="14.25"/>
-    <row r="130" ht="14.25"/>
-    <row r="131" ht="14.25"/>
-    <row r="132" ht="14.25"/>
-    <row r="133" ht="14.25"/>
-    <row r="134" ht="14.25"/>
-    <row r="135" ht="14.25"/>
-    <row r="136" ht="14.25"/>
-    <row r="137" ht="14.25"/>
-    <row r="138" ht="14.25"/>
-    <row r="139" ht="14.25"/>
-    <row r="140" ht="14.25"/>
-    <row r="141" ht="14.25"/>
-    <row r="142" ht="14.25"/>
-    <row r="143" ht="14.25"/>
-    <row r="144" ht="14.25"/>
-    <row r="145" ht="14.25"/>
-    <row r="146" ht="14.25"/>
-    <row r="147" ht="14.25"/>
-    <row r="148" ht="14.25"/>
-    <row r="149" ht="14.25"/>
-    <row r="150" ht="14.25"/>
-    <row r="151" ht="14.25"/>
-    <row r="152" ht="14.25"/>
+    <row r="118" ht="14.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+    </row>
+    <row r="119" ht="14.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+    </row>
+    <row r="120" ht="14.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1">
+        <v>1</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" ht="14.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="6">
+        <v>2</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" ht="14.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1">
+        <v>3</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+    </row>
+    <row r="123" ht="14.25">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1">
+        <v>4</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+    </row>
+    <row r="124" ht="14.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="6">
+        <v>5</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+    </row>
+    <row r="125" ht="14.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1">
+        <v>6</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+    </row>
+    <row r="126" ht="14.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1">
+        <v>7</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" ht="14.25">
+      <c r="A127" s="1"/>
+      <c r="B127" s="6">
+        <v>8</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+    </row>
+    <row r="128" ht="14.25">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+    </row>
+    <row r="130" ht="14.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1">
+        <v>1</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+    </row>
+    <row r="131" ht="14.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="6">
+        <v>2</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+    </row>
+    <row r="132" ht="14.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1">
+        <v>3</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+    </row>
+    <row r="133" ht="14.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" ht="14.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="6">
+        <v>5</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+    </row>
+    <row r="135" ht="14.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1">
+        <v>6</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+    </row>
+    <row r="136" ht="14.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1">
+        <v>7</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+    </row>
+    <row r="137" ht="14.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="6">
+        <v>8</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+    </row>
+    <row r="138" ht="14.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+    </row>
+    <row r="139" ht="14.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+    </row>
+    <row r="140" ht="14.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+    </row>
+    <row r="141" ht="14.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1">
+        <v>1</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+    </row>
+    <row r="142" ht="14.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="6">
+        <v>2</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+    </row>
+    <row r="143" ht="14.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1">
+        <v>3</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+    </row>
+    <row r="144" ht="14.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1">
+        <v>4</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+    </row>
+    <row r="145" ht="14.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="6">
+        <v>5</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+    </row>
+    <row r="146" ht="14.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1">
+        <v>6</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+    </row>
+    <row r="147" ht="14.25">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+    </row>
+    <row r="148" ht="14.25">
+      <c r="A148" s="1"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+    </row>
+    <row r="149" ht="14.25">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+    </row>
+    <row r="150" ht="14.25">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+    </row>
+    <row r="151" ht="14.25">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+    </row>
+    <row r="152" ht="14.25">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+    </row>
     <row r="153" ht="14.25"/>
     <row r="154" ht="14.25"/>
     <row r="155" ht="14.25"/>

</xml_diff>